<commit_message>
report updates, only need "interesting bits of code", "man in middle attacks and DDOS protection", for the technology report
</commit_message>
<xml_diff>
--- a/project/Report/tech-progr/ProgrammingTechnology-ReportTasks.xlsx
+++ b/project/Report/tech-progr/ProgrammingTechnology-ReportTasks.xlsx
@@ -117,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,12 +136,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -166,10 +160,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -464,7 +454,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F9" sqref="F9:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,13 +472,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -497,14 +487,14 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -513,12 +503,12 @@
       <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -527,12 +517,12 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -541,12 +531,12 @@
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -555,12 +545,12 @@
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -569,12 +559,12 @@
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -583,12 +573,12 @@
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -597,28 +587,28 @@
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="F9" s="9" t="s">
+      <c r="C9" s="8"/>
+      <c r="F9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -627,12 +617,12 @@
       <c r="B11" s="5">
         <v>2.4</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -641,12 +631,12 @@
       <c r="B12" s="5">
         <v>2.5</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -655,26 +645,26 @@
       <c r="B13" s="3">
         <v>2.6</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="3">
         <v>2.7</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -683,19 +673,19 @@
       <c r="B15" s="5">
         <v>3</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -704,14 +694,14 @@
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -720,12 +710,12 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -734,12 +724,12 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -748,26 +738,26 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>